<commit_message>
Added option for dz=12mm
</commit_message>
<xml_diff>
--- a/mseplots_amp_sbmir.xlsx
+++ b/mseplots_amp_sbmir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darkroom\Joshua\mainlatest\FRCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214A7FAD-3603-479F-A855-DDF478F31685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F68EA-3FEA-4AD9-90A8-9BBB8FE095C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{181DF939-437F-4801-A272-FB7E58917727}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{039AD695-1360-4545-AAB7-351913564F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838AAD26-D14A-42FB-A291-2B648F2C1DCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49688E9C-04A7-4118-A8CC-755F3FBFC571}">
   <dimension ref="A2:C171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -415,10 +415,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5.5706790986700989</v>
+        <v>10.560652069627087</v>
       </c>
       <c r="C2">
-        <v>4.5650211617135099</v>
+        <v>9.8574093329804366</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,10 +426,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5.13259838988757</v>
+        <v>10.086981386205785</v>
       </c>
       <c r="C3">
-        <v>4.2343124875797731</v>
+        <v>9.5860446218238593</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.9113121974754979</v>
+        <v>9.8587501894022882</v>
       </c>
       <c r="C4">
-        <v>4.0516018955699105</v>
+        <v>9.4869121092482835</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,10 +448,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.7935967397444488</v>
+        <v>9.7441330258133441</v>
       </c>
       <c r="C5">
-        <v>3.9059972964926515</v>
+        <v>9.4141278971085516</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,10 +459,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4.6981766541577175</v>
+        <v>9.646986130090843</v>
       </c>
       <c r="C6">
-        <v>3.792662800229837</v>
+        <v>9.353141097098117</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,10 +470,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.6226533146884048</v>
+        <v>9.5487241836380434</v>
       </c>
       <c r="C7">
-        <v>3.7140137278324765</v>
+        <v>9.2926389125566331</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,10 +481,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.5614987824388944</v>
+        <v>9.4803833172195606</v>
       </c>
       <c r="C8">
-        <v>3.6457079803384609</v>
+        <v>9.2394974708771525</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,10 +492,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.5114973558479337</v>
+        <v>9.4317712108126379</v>
       </c>
       <c r="C9">
-        <v>3.5798624487386967</v>
+        <v>9.1786173844608303</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,10 +503,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4.4611509836029946</v>
+        <v>9.3924463095875801</v>
       </c>
       <c r="C10">
-        <v>3.5223925271391359</v>
+        <v>9.0887422589830251</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,10 +514,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.4189451377261619</v>
+        <v>9.3461825204923095</v>
       </c>
       <c r="C11">
-        <v>3.488096516294219</v>
+        <v>8.9719099088676426</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,10 +525,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4.3747457624701909</v>
+        <v>9.3217134852629968</v>
       </c>
       <c r="C12">
-        <v>3.4583802989709067</v>
+        <v>8.8601865018979566</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,10 +536,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4.3344313356526945</v>
+        <v>9.296654579140684</v>
       </c>
       <c r="C13">
-        <v>3.4205670873082603</v>
+        <v>8.7370022316471374</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,10 +547,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.2950558816636661</v>
+        <v>9.2767147707011297</v>
       </c>
       <c r="C14">
-        <v>3.3893071007910787</v>
+        <v>8.617214391426737</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,10 +558,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4.2530947951999165</v>
+        <v>9.2417064537311173</v>
       </c>
       <c r="C15">
-        <v>3.3708334732083269</v>
+        <v>8.5040501757495441</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,10 +569,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4.2127676332542476</v>
+        <v>9.232396537011196</v>
       </c>
       <c r="C16">
-        <v>3.3534778695423508</v>
+        <v>8.4090233278396429</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,10 +580,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.1724284005956447</v>
+        <v>9.2065123045903956</v>
       </c>
       <c r="C17">
-        <v>3.3354065125423937</v>
+        <v>8.3376143528812285</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,10 +591,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4.1296030469098852</v>
+        <v>9.1758179867380552</v>
       </c>
       <c r="C18">
-        <v>3.3219494528838385</v>
+        <v>8.2703998480611904</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,10 +602,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4.0919519596689318</v>
+        <v>9.1606487565274595</v>
       </c>
       <c r="C19">
-        <v>3.3045012588360221</v>
+        <v>8.1961618641705787</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,10 +613,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4.0502149786118284</v>
+        <v>9.1411263328316501</v>
       </c>
       <c r="C20">
-        <v>3.2950282428881899</v>
+        <v>8.1235335586363551</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,10 +624,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4.007941274504895</v>
+        <v>9.1182627260556064</v>
       </c>
       <c r="C21">
-        <v>3.2865418914970843</v>
+        <v>8.0486140044147927</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,10 +635,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>3.9716595553467067</v>
+        <v>9.0960555940064403</v>
       </c>
       <c r="C22">
-        <v>3.2785519180292586</v>
+        <v>7.9821024070341755</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,10 +646,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>3.9311882123383919</v>
+        <v>9.0659772277762389</v>
       </c>
       <c r="C23">
-        <v>3.2731285268422239</v>
+        <v>7.906871677543883</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,10 +657,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>3.8962636299230189</v>
+        <v>9.0383597511325142</v>
       </c>
       <c r="C24">
-        <v>3.2689719083291298</v>
+        <v>7.8232147001774992</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,10 +668,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.8649263167586794</v>
+        <v>9.0153420899600434</v>
       </c>
       <c r="C25">
-        <v>3.2629232503796164</v>
+        <v>7.7429673835441148</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,10 +679,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>3.831760399712556</v>
+        <v>8.9993017166898213</v>
       </c>
       <c r="C26">
-        <v>3.2521354875912039</v>
+        <v>7.6439522832456088</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,10 +690,10 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>3.804832281839857</v>
+        <v>8.9724244914878302</v>
       </c>
       <c r="C27">
-        <v>3.2422950575795086</v>
+        <v>7.5494662688889216</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,10 +701,10 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>3.7765489597849604</v>
+        <v>8.9434125941186196</v>
       </c>
       <c r="C28">
-        <v>3.2306453270122724</v>
+        <v>7.4760661538121269</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,10 +712,10 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>3.7518251097140047</v>
+        <v>8.9168154402028907</v>
       </c>
       <c r="C29">
-        <v>3.2239798702812594</v>
+        <v>7.4155387684684912</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,10 +723,10 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>3.7293035169781348</v>
+        <v>8.9000120695401996</v>
       </c>
       <c r="C30">
-        <v>3.2196557008481501</v>
+        <v>7.375945707105906</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,10 +734,10 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>3.7076235878746933</v>
+        <v>8.8636620587797861</v>
       </c>
       <c r="C31">
-        <v>3.2165220063640483</v>
+        <v>7.3386275041759532</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,10 +745,10 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>3.6887594912336907</v>
+        <v>8.8417000260002538</v>
       </c>
       <c r="C32">
-        <v>3.213455026261653</v>
+        <v>7.3022281564753948</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,10 +756,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>3.675526342950469</v>
+        <v>8.822662027985638</v>
       </c>
       <c r="C33">
-        <v>3.2094398898763985</v>
+        <v>7.2656817666802738</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,10 +767,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>3.6600614325525087</v>
+        <v>8.798188303771326</v>
       </c>
       <c r="C34">
-        <v>3.2064231474044931</v>
+        <v>7.2416881033238694</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,10 +778,10 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>3.6459102494866484</v>
+        <v>8.7544157729870999</v>
       </c>
       <c r="C35">
-        <v>3.2029251784858799</v>
+        <v>7.224625934660069</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,10 +789,10 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>3.634012895307456</v>
+        <v>8.7359969493964904</v>
       </c>
       <c r="C36">
-        <v>3.1987527541060503</v>
+        <v>7.2098835721315933</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,10 +800,10 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>3.6219049200973163</v>
+        <v>8.7024336342611015</v>
       </c>
       <c r="C37">
-        <v>3.1955803614368459</v>
+        <v>7.1973800671029267</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,10 +811,10 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>3.6122735124099448</v>
+        <v>8.6709174167208722</v>
       </c>
       <c r="C38">
-        <v>3.193225377822003</v>
+        <v>7.1839139607851958</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,10 +822,10 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>3.6039496483845528</v>
+        <v>8.6471907353405957</v>
       </c>
       <c r="C39">
-        <v>3.1912577098986707</v>
+        <v>7.1713778688456067</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,10 +833,10 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>3.5941281193791794</v>
+        <v>8.6073433436887772</v>
       </c>
       <c r="C40">
-        <v>3.1900018979575271</v>
+        <v>7.1612370010896464</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,10 +844,10 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>3.5864768688923414</v>
+        <v>8.573690368012965</v>
       </c>
       <c r="C41">
-        <v>3.1888411407358648</v>
+        <v>7.1543163250218047</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,10 +855,10 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>3.581636982177987</v>
+        <v>8.5466104693897158</v>
       </c>
       <c r="C42">
-        <v>3.1877112672170607</v>
+        <v>7.1502860492558531</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,10 +866,10 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>3.5740617711998883</v>
+        <v>8.5144620562002213</v>
       </c>
       <c r="C43">
-        <v>3.1859367684258895</v>
+        <v>7.1472555375809899</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,10 +877,10 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>3.5631794739279532</v>
+        <v>8.492892778710571</v>
       </c>
       <c r="C44">
-        <v>3.1839646661109837</v>
+        <v>7.1443985290918386</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,10 +888,10 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>3.5556217068971163</v>
+        <v>8.4721240130805366</v>
       </c>
       <c r="C45">
-        <v>3.1814789546555091</v>
+        <v>7.1413035363398434</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,10 +899,10 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>3.5494023921882754</v>
+        <v>8.4473158715928793</v>
       </c>
       <c r="C46">
-        <v>3.1766060860546217</v>
+        <v>7.1378092167061888</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,10 +910,10 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>3.5438567721713112</v>
+        <v>8.4193158919825457</v>
       </c>
       <c r="C47">
-        <v>3.1744277437540172</v>
+        <v>7.1342439018189188</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,10 +921,10 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>3.5368924935488333</v>
+        <v>8.3900540084173816</v>
       </c>
       <c r="C48">
-        <v>3.1713216687644956</v>
+        <v>7.1307078052941915</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,10 +932,10 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>3.5280328113898531</v>
+        <v>8.3574347052878579</v>
       </c>
       <c r="C49">
-        <v>3.1624636247841886</v>
+        <v>7.1283975258945418</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,10 +943,10 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>3.5192968249848984</v>
+        <v>8.3325882294277083</v>
       </c>
       <c r="C50">
-        <v>3.1540810070220937</v>
+        <v>7.127054916907607</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,10 +954,10 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>3.5120493362403904</v>
+        <v>8.3092907436551577</v>
       </c>
       <c r="C51">
-        <v>3.1510193119402516</v>
+        <v>7.1246050800880747</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,10 +965,10 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>3.5060555422879518</v>
+        <v>8.2826982392629489</v>
       </c>
       <c r="C52">
-        <v>3.1479421418916469</v>
+        <v>7.1215611854885514</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,10 +976,10 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>3.4983651123151298</v>
+        <v>8.2575176787943683</v>
       </c>
       <c r="C53">
-        <v>3.1441652490345398</v>
+        <v>7.1189044519225604</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,10 +987,10 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>3.4897027743429532</v>
+        <v>8.2309254686724813</v>
       </c>
       <c r="C54">
-        <v>3.1370352830667851</v>
+        <v>7.117942916294778</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,10 +998,10 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>3.4829462767991322</v>
+        <v>8.2043136101406979</v>
       </c>
       <c r="C55">
-        <v>3.1330964428164441</v>
+        <v>7.1168513579009751</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,10 +1009,10 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>3.4783957635708074</v>
+        <v>8.187349804299437</v>
       </c>
       <c r="C56">
-        <v>3.1306699375352265</v>
+        <v>7.11413303664993</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,10 +1020,10 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>3.4731577462901946</v>
+        <v>8.1613161764547133</v>
       </c>
       <c r="C57">
-        <v>3.1288118218595309</v>
+        <v>7.1112759134661578</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,10 +1031,10 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>3.4706518344424131</v>
+        <v>8.1342790133724652</v>
       </c>
       <c r="C58">
-        <v>3.1268698747049632</v>
+        <v>7.1103641597786238</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,10 +1042,10 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>3.4677872182654688</v>
+        <v>8.1016872291322741</v>
       </c>
       <c r="C59">
-        <v>3.1252008166701661</v>
+        <v>7.10868126623095</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,10 +1053,10 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>3.4669054006567808</v>
+        <v>8.0796010091253159</v>
       </c>
       <c r="C60">
-        <v>3.1233353041731324</v>
+        <v>7.1064432021886956</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,10 +1064,10 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>3.4634875782858359</v>
+        <v>8.0613767839507631</v>
       </c>
       <c r="C61">
-        <v>3.1214128772762568</v>
+        <v>7.104666276218933</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,10 +1075,10 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>3.4569325148054855</v>
+        <v>8.0371320774839621</v>
       </c>
       <c r="C62">
-        <v>3.1198946609884568</v>
+        <v>7.1041120353136424</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>3.4492595824696162</v>
+        <v>8.0173712174335918</v>
       </c>
       <c r="C63">
-        <v>3.1182442227316467</v>
+        <v>7.1022109756949181</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,10 +1097,10 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>3.4439847757144717</v>
+        <v>7.9993573863390983</v>
       </c>
       <c r="C64">
-        <v>3.1170951070602384</v>
+        <v>7.1020673396472738</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,10 +1108,10 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>3.4421727410269591</v>
+        <v>7.9767602929068859</v>
       </c>
       <c r="C65">
-        <v>3.1153328456899647</v>
+        <v>7.1017318561461957</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,10 +1119,10 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>3.4405564223348186</v>
+        <v>7.9522541730100453</v>
       </c>
       <c r="C66">
-        <v>3.1129074398458125</v>
+        <v>7.1006667152757839</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,10 +1130,10 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>3.4371821926057127</v>
+        <v>7.9306923392218183</v>
       </c>
       <c r="C67">
-        <v>3.1115907800029539</v>
+        <v>7.0994197391959597</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,10 +1141,10 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>3.4369251372209355</v>
+        <v>7.9052127525389562</v>
       </c>
       <c r="C68">
-        <v>3.110198944935024</v>
+        <v>7.0980995941391418</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,10 +1152,10 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>3.4342646439132012</v>
+        <v>7.8863252143290072</v>
       </c>
       <c r="C69">
-        <v>3.1070026140615439</v>
+        <v>7.0974375642846326</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,10 +1163,10 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>3.4349338723677607</v>
+        <v>7.8688115426583849</v>
       </c>
       <c r="C70">
-        <v>3.104883085027565</v>
+        <v>7.0967290955731945</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,10 +1174,10 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>3.4310149646376242</v>
+        <v>7.8525307190762215</v>
       </c>
       <c r="C71">
-        <v>3.1005033991901376</v>
+        <v>7.096610227885499</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>3.4292014800063155</v>
+        <v>7.8354214551108168</v>
       </c>
       <c r="C72">
-        <v>3.0971016286549569</v>
+        <v>7.0965977189485727</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,10 +1196,10 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>3.4306056017606226</v>
+        <v>7.820388283845543</v>
       </c>
       <c r="C73">
-        <v>3.0964914757046405</v>
+        <v>7.0973737303112667</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,10 +1207,10 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>3.4274898109083982</v>
+        <v>7.7904892327891471</v>
       </c>
       <c r="C74">
-        <v>3.0957991763770258</v>
+        <v>7.0969150495003968</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>3.4241089550913677</v>
+        <v>7.7722972311888467</v>
       </c>
       <c r="C75">
-        <v>3.0948902857692233</v>
+        <v>7.0951479929693804</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>3.4222060548616771</v>
+        <v>7.7558601436015042</v>
       </c>
       <c r="C76">
-        <v>3.094231310544556</v>
+        <v>7.0931173024416534</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,10 +1240,10 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>3.4205917056034241</v>
+        <v>7.7357195874259528</v>
       </c>
       <c r="C77">
-        <v>3.0938490884779566</v>
+        <v>7.0914042857047024</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,10 +1251,10 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>3.4188007835795147</v>
+        <v>7.7218395649447098</v>
       </c>
       <c r="C78">
-        <v>3.0935949802296765</v>
+        <v>7.0892925440573844</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,10 +1262,10 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>3.4188162473147146</v>
+        <v>7.7108530734342393</v>
       </c>
       <c r="C79">
-        <v>3.093457005282326</v>
+        <v>7.0874886873103149</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,10 +1273,10 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>3.4173976982011993</v>
+        <v>7.7003379201313233</v>
       </c>
       <c r="C80">
-        <v>3.0932450300312184</v>
+        <v>7.0864135189663333</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,10 +1284,10 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>3.4147999510369802</v>
+        <v>7.6929584630795329</v>
       </c>
       <c r="C81">
-        <v>3.0926816447980117</v>
+        <v>7.0853460612319257</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,10 +1295,10 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>3.4116008831835445</v>
+        <v>7.6816951994065468</v>
       </c>
       <c r="C82">
-        <v>3.0922650001287142</v>
+        <v>7.0840343654352207</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,10 +1306,10 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>3.4111450486377941</v>
+        <v>7.6745155286007245</v>
       </c>
       <c r="C83">
-        <v>3.0916624704754141</v>
+        <v>7.0823743838662132</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,10 +1317,10 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>3.4098811476691626</v>
+        <v>7.6663119437504985</v>
       </c>
       <c r="C84">
-        <v>3.0908166684589049</v>
+        <v>7.079975296541007</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1328,10 +1328,10 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>3.4053466114860607</v>
+        <v>7.6538115312077446</v>
       </c>
       <c r="C85">
-        <v>3.0905685966026772</v>
+        <v>7.077450131319341</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,10 +1339,10 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>3.3996208398925978</v>
+        <v>7.6406775109786329</v>
       </c>
       <c r="C86">
-        <v>3.0900330735564592</v>
+        <v>7.0753764197398459</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>3.3978483292719095</v>
+        <v>7.6307007026948339</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>3.3957675573101422</v>
+        <v>7.6213614791340341</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>3.3944984876970095</v>
+        <v>7.6088371293420849</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>3.3937614250029724</v>
+        <v>7.5944228021795217</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>3.3935985594952705</v>
+        <v>7.5759171739219164</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>3.3917585226496909</v>
+        <v>7.5707632037204853</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>3.3922540713910099</v>
+        <v>7.5492801640765652</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>3.3918678776573632</v>
+        <v>7.533253556612312</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>3.3941834802897977</v>
+        <v>7.5191542147238968</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>3.3922807745831789</v>
+        <v>7.5056082031234856</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>3.3901966576705047</v>
+        <v>7.4921110027410087</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>3.3917618515657635</v>
+        <v>7.4762642833129078</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>3.390295900314678</v>
+        <v>7.464736407933378</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>3.3919289693143693</v>
+        <v>7.4681392271234559</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>3.3920859753285311</v>
+        <v>7.4586843369385436</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>3.3920593009087638</v>
+        <v>7.4491038147449373</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>3.3908635606525395</v>
+        <v>7.4357410128470267</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>3.3915388670734101</v>
+        <v>7.4240603917873527</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>3.391323890215344</v>
+        <v>7.4206568056540938</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>3.3915707698612256</v>
+        <v>7.4086980806134237</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>3.3914053448948094</v>
+        <v>7.4021565440670223</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>3.390348220405107</v>
+        <v>7.3948092477604179</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>3.3894400823837305</v>
+        <v>7.3857488149176449</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>3.3885082278749126</v>
+        <v>7.3816584296953396</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>3.3885344926199195</v>
+        <v>7.3765753738616517</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>3.3883640320166521</v>
+        <v>7.3635313073567179</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>3.3869628378169376</v>
+        <v>7.3560332053087505</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>3.3891721780693058</v>
+        <v>7.3477375801006026</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>3.3888254212915481</v>
+        <v>7.3478671144498344</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>3.3889523546687519</v>
+        <v>7.3370635770438142</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>3.3883566410579591</v>
+        <v>7.330893860690459</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>3.3887591019068335</v>
+        <v>7.3256077560332526</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>3.3871740658230367</v>
+        <v>7.3226959552139466</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>3.3883354917082205</v>
+        <v>7.3183429639529542</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,7 +1622,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>3.3891945630031892</v>
+        <v>7.3073352708677453</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>3.3887053263313782</v>
+        <v>7.3030384988227501</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>3.3884670008846332</v>
+        <v>7.3026091875140189</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>3.3868587970705879</v>
+        <v>7.3019942409749907</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>3.386283038848481</v>
+        <v>7.3022473639128167</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>3.385092626006716</v>
+        <v>7.300130377859869</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>3.3854795576052128</v>
+        <v>7.3026978414714065</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -1678,7 +1678,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>3.3846591667400281</v>
+        <v>7.2951500103547939</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>3.3856641687133622</v>
+        <v>7.2918486191817529</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>3.3856319438740807</v>
+        <v>7.2872996224150439</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>3.3860270279444027</v>
+        <v>7.2867526710013841</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>3.3861475972130055</v>
+        <v>7.2839883882099938</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>3.3862343773308838</v>
+        <v>7.2819350967537835</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1726,7 +1726,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>3.3877174755500676</v>
+        <v>7.2788675844286548</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>3.3872839177589693</v>
+        <v>7.2794298502443215</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1742,7 +1742,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>3.3876220665933725</v>
+        <v>7.2816243828723008</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>3.3886400571776765</v>
+        <v>7.2850059923024677</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>3.3886024426945505</v>
+        <v>7.2897882381889261</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,7 +1766,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>3.3867474272493991</v>
+        <v>7.2863851875219465</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -1774,7 +1774,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>3.3884439419295465</v>
+        <v>7.2818245137461881</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -1782,7 +1782,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>3.3890447283673213</v>
+        <v>7.2763873298924704</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -1790,7 +1790,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>3.3870262046618103</v>
+        <v>7.2738690567839877</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -1798,7 +1798,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>3.3869014057069533</v>
+        <v>7.2723217898976591</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,7 +1806,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>3.3861064608526319</v>
+        <v>7.2725066719543134</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -1814,7 +1814,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>3.3851947763382277</v>
+        <v>7.2793788480307349</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -1822,7 +1822,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>3.3835761749211275</v>
+        <v>7.2767442892210958</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -1830,7 +1830,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>3.3842667568127616</v>
+        <v>7.2700252834732497</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>3.3832642674299307</v>
+        <v>7.2693263510628148</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -1846,7 +1846,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>3.3840413228134798</v>
+        <v>7.2744109615506423</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -1854,7 +1854,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>3.3834455976353648</v>
+        <v>7.2705348383634689</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>3.3831117650830347</v>
+        <v>7.2733825038670235</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>3.38336269448736</v>
+        <v>7.2728314404071455</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>3.3840585562203271</v>
+        <v>7.2749863692358687</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -1886,7 +1886,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>3.3830034614222537</v>
+        <v>7.2777058639532752</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>3.3809718891709304</v>
+        <v>7.2768986736000114</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>3.3812412598248964</v>
+        <v>7.2771914071989707</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>3.3800686392592265</v>
+        <v>7.2752820022896056</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>3.3813356415790081</v>
+        <v>7.2732990941863287</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>3.382536332290381</v>
+        <v>7.2688658512660247</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,7 +1934,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>3.3821033993568195</v>
+        <v>7.2726524174223757</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>3.3825680680502739</v>
+        <v>7.2733878537591554</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>3.3804001278383855</v>
+        <v>7.2740458880435028</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>3.3780481603072183</v>
+        <v>7.2703100977088591</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>3.377665919565179</v>
+        <v>7.2710412190868006</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>3.3794879409367193</v>
+        <v>7.2675839936352373</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>3.3791385536441738</v>
+        <v>7.2686439641929734</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>3.3799627075820604</v>
+        <v>7.271529924856611</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>3.3801309999536251</v>
+        <v>7.2719208632927845</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>3.378971415521395</v>
+        <v>7.2662642074621964</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>3.3776054215113924</v>
+        <v>7.2644406315905519</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>3.3785241418511291</v>
+        <v>7.261390149377573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>